<commit_message>
test data for add genes
</commit_message>
<xml_diff>
--- a/src/crispr_screen_viewer/tests/test_data/exorcise_style/test1/re/det/test1.xlsx
+++ b/src/crispr_screen_viewer/tests/test_data/exorcise_style/test1/re/det/test1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas03/python_projects/crispr_screen_viewer/src/crispr_screen_viewer/test_data/exorcise_style/test1/re/det/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas03/python_projects/crispr_screen_viewer/src/crispr_screen_viewer/tests/test_data/exorcise_style/test1/re/det/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D36D9C-CB12-4D44-B4C4-F014D5A4FDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC34C49-598F-A943-AEB0-42AF71AF523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="33500" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>Library</t>
   </si>
@@ -429,6 +429,12 @@
   </si>
   <si>
     <t>re/res</t>
+  </si>
+  <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>Human</t>
   </si>
 </sst>
 </file>
@@ -1493,10 +1499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1591,6 +1597,14 @@
       </c>
       <c r="B11" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20">
+      <c r="A12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>